<commit_message>
Renombrar y nuevo code
</commit_message>
<xml_diff>
--- a/Data/Puntos riesgo país.xlsx
+++ b/Data/Puntos riesgo país.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://estudusfqedu-my.sharepoint.com/personal/esoria_estud_usfq_edu_ec/Documents/Escritorio/Quantificador/RiesgopaisSoria/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://estudusfqedu-my.sharepoint.com/personal/esoria_estud_usfq_edu_ec/Documents/Escritorio/Quantificador/RiesgopaisSoria/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{9C9838B8-88AE-47BC-8456-EBB70C85706E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA464B89-C21B-49ED-8F2C-E890BDA33212}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{9C9838B8-88AE-47BC-8456-EBB70C85706E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F50FA094-A0F5-4C5D-8ED2-B8AF199CE5B4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{AC08FCD3-5F89-4E94-8ACC-8D65B117AB27}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>A fin de período</t>
   </si>
@@ -46,24 +46,13 @@
   <si>
     <t>Periodo</t>
   </si>
-  <si>
-    <t>Puntos del riesgo país</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -111,29 +100,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -149,6 +135,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -448,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AC7F0A-92D3-445F-85C6-0A8224A8026B}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="53" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:B1048576"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -461,613 +451,603 @@
     <col min="3" max="3" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
+      <c r="A2" s="6">
+        <v>43466</v>
+      </c>
+      <c r="B2" s="4">
+        <v>690</v>
+      </c>
+      <c r="C2" s="4">
+        <v>712</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
-        <v>43466</v>
+        <v>43497</v>
       </c>
       <c r="B3" s="4">
-        <v>690</v>
+        <v>584</v>
       </c>
       <c r="C3" s="4">
-        <v>712</v>
+        <v>658</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
-        <v>43497</v>
+        <v>43525</v>
       </c>
       <c r="B4" s="4">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="C4" s="4">
-        <v>658</v>
+        <v>612</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
-        <v>43525</v>
+        <v>43556</v>
       </c>
       <c r="B5" s="4">
-        <v>592</v>
+        <v>560</v>
       </c>
       <c r="C5" s="4">
-        <v>612</v>
+        <v>552</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
-        <v>43556</v>
+        <v>43586</v>
       </c>
       <c r="B6" s="4">
-        <v>560</v>
+        <v>619</v>
       </c>
       <c r="C6" s="4">
-        <v>552</v>
+        <v>573</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
-        <v>43586</v>
+        <v>43617</v>
       </c>
       <c r="B7" s="4">
-        <v>619</v>
+        <v>580</v>
       </c>
       <c r="C7" s="4">
-        <v>573</v>
+        <v>590</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
-        <v>43617</v>
+        <v>43647</v>
       </c>
       <c r="B8" s="4">
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="C8" s="4">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
-        <v>43647</v>
+        <v>43678</v>
       </c>
       <c r="B9" s="4">
-        <v>603</v>
+        <v>705</v>
       </c>
       <c r="C9" s="4">
-        <v>578</v>
+        <v>702</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
-        <v>43678</v>
+        <v>43709</v>
       </c>
       <c r="B10" s="4">
-        <v>705</v>
+        <v>677</v>
       </c>
       <c r="C10" s="4">
-        <v>702</v>
+        <v>648</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
-        <v>43709</v>
+        <v>43739</v>
       </c>
       <c r="B11" s="4">
-        <v>677</v>
+        <v>789</v>
       </c>
       <c r="C11" s="4">
-        <v>648</v>
+        <v>763</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
-        <v>43739</v>
+        <v>43770</v>
       </c>
       <c r="B12" s="4">
-        <v>789</v>
+        <v>1146</v>
       </c>
       <c r="C12" s="4">
-        <v>763</v>
+        <v>979</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
-        <v>43770</v>
+        <v>43800</v>
       </c>
       <c r="B13" s="4">
-        <v>1146</v>
+        <v>826</v>
       </c>
       <c r="C13" s="4">
-        <v>979</v>
+        <v>938</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
-        <v>43800</v>
+        <v>43831</v>
       </c>
       <c r="B14" s="4">
-        <v>826</v>
+        <v>1018</v>
       </c>
       <c r="C14" s="4">
-        <v>938</v>
+        <v>859</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
-        <v>43831</v>
+        <v>43862</v>
       </c>
       <c r="B15" s="4">
-        <v>1018</v>
+        <v>1466</v>
       </c>
       <c r="C15" s="4">
-        <v>859</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="B16" s="4">
-        <v>1466</v>
+        <v>4553</v>
       </c>
       <c r="C16" s="4">
-        <v>1180</v>
+        <v>3580</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
-        <v>43891</v>
+        <v>43922</v>
       </c>
       <c r="B17" s="4">
-        <v>4553</v>
+        <v>5129</v>
       </c>
       <c r="C17" s="4">
-        <v>3580</v>
+        <v>5033</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
-        <v>43922</v>
+        <v>43952</v>
       </c>
       <c r="B18" s="4">
-        <v>5129</v>
+        <v>3907</v>
       </c>
       <c r="C18" s="4">
-        <v>5033</v>
+        <v>4305</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
-        <v>43952</v>
+        <v>43983</v>
       </c>
       <c r="B19" s="4">
-        <v>3907</v>
+        <v>3373</v>
       </c>
       <c r="C19" s="4">
-        <v>4305</v>
+        <v>3287</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
-        <v>43983</v>
+        <v>44013</v>
       </c>
       <c r="B20" s="4">
-        <v>3373</v>
+        <v>2755</v>
       </c>
       <c r="C20" s="4">
-        <v>3287</v>
+        <v>2862</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
-        <v>44013</v>
+        <v>44044</v>
       </c>
       <c r="B21" s="4">
-        <v>2755</v>
+        <v>2813</v>
       </c>
       <c r="C21" s="4">
-        <v>2862</v>
+        <v>2780</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
-        <v>44044</v>
+        <v>44075</v>
       </c>
       <c r="B22" s="4">
-        <v>2813</v>
+        <v>1015</v>
       </c>
       <c r="C22" s="4">
-        <v>2780</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
-        <v>44075</v>
+        <v>44105</v>
       </c>
       <c r="B23" s="4">
-        <v>1015</v>
+        <v>1029</v>
       </c>
       <c r="C23" s="4">
-        <v>1413</v>
+        <v>983</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
-        <v>44105</v>
+        <v>44136</v>
       </c>
       <c r="B24" s="4">
-        <v>1029</v>
+        <v>1065</v>
       </c>
       <c r="C24" s="4">
-        <v>983</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
-        <v>44136</v>
+        <v>44166</v>
       </c>
       <c r="B25" s="4">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="C25" s="4">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
-        <v>44166</v>
+        <v>44197</v>
       </c>
       <c r="B26" s="4">
-        <v>1062</v>
+        <v>1273</v>
       </c>
       <c r="C26" s="4">
-        <v>1041</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
-        <v>44197</v>
+        <v>44228</v>
       </c>
       <c r="B27" s="4">
-        <v>1273</v>
+        <v>1226</v>
       </c>
       <c r="C27" s="4">
-        <v>1182</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
-        <v>44228</v>
+        <v>44256</v>
       </c>
       <c r="B28" s="4">
-        <v>1226</v>
+        <v>1201</v>
       </c>
       <c r="C28" s="4">
-        <v>1202</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="6">
-        <v>44256</v>
+        <v>44287</v>
       </c>
       <c r="B29" s="4">
-        <v>1201</v>
+        <v>764</v>
       </c>
       <c r="C29" s="4">
-        <v>1264</v>
+        <v>937</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
-        <v>44287</v>
+        <v>44317</v>
       </c>
       <c r="B30" s="4">
-        <v>764</v>
+        <v>730</v>
       </c>
       <c r="C30" s="4">
-        <v>937</v>
+        <v>735</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="6">
-        <v>44317</v>
+        <v>44348</v>
       </c>
       <c r="B31" s="4">
-        <v>730</v>
+        <v>776</v>
       </c>
       <c r="C31" s="4">
-        <v>735</v>
+        <v>757</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
-        <v>44348</v>
+        <v>44378</v>
       </c>
       <c r="B32" s="4">
-        <v>776</v>
+        <v>790</v>
       </c>
       <c r="C32" s="4">
-        <v>757</v>
+        <v>777</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
-        <v>44378</v>
+        <v>44409</v>
       </c>
       <c r="B33" s="4">
-        <v>790</v>
+        <v>751</v>
       </c>
       <c r="C33" s="4">
-        <v>777</v>
+        <v>793</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="6">
-        <v>44409</v>
+        <v>44440</v>
       </c>
       <c r="B34" s="4">
-        <v>751</v>
+        <v>835</v>
       </c>
       <c r="C34" s="4">
-        <v>793</v>
+        <v>797</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
-        <v>44440</v>
+        <v>44470</v>
       </c>
       <c r="B35" s="4">
-        <v>835</v>
+        <v>847</v>
       </c>
       <c r="C35" s="4">
-        <v>797</v>
+        <v>825</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="6">
-        <v>44470</v>
+        <v>44501</v>
       </c>
       <c r="B36" s="4">
-        <v>847</v>
+        <v>891</v>
       </c>
       <c r="C36" s="4">
-        <v>825</v>
+        <v>834</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
-        <v>44501</v>
+        <v>44531</v>
       </c>
       <c r="B37" s="4">
-        <v>891</v>
+        <v>869</v>
       </c>
       <c r="C37" s="4">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="6">
-        <v>44531</v>
+        <v>44562</v>
       </c>
       <c r="B38" s="4">
-        <v>869</v>
+        <v>768</v>
       </c>
       <c r="C38" s="4">
-        <v>867</v>
+        <v>818</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="6">
-        <v>44562</v>
+        <v>44593</v>
       </c>
       <c r="B39" s="4">
-        <v>768</v>
+        <v>755</v>
       </c>
       <c r="C39" s="4">
-        <v>818</v>
+        <v>761</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="6">
-        <v>44593</v>
+        <v>44621</v>
       </c>
       <c r="B40" s="4">
-        <v>755</v>
+        <v>810</v>
       </c>
       <c r="C40" s="4">
-        <v>761</v>
+        <v>792</v>
       </c>
     </row>
     <row r="41" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="6">
-        <v>44621</v>
+        <v>44652</v>
       </c>
       <c r="B41" s="4">
-        <v>810</v>
+        <v>816</v>
       </c>
       <c r="C41" s="4">
-        <v>792</v>
+        <v>803</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="6">
-        <v>44652</v>
+        <v>44682</v>
       </c>
       <c r="B42" s="4">
-        <v>816</v>
+        <v>802</v>
       </c>
       <c r="C42" s="4">
-        <v>803</v>
+        <v>805</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="6">
-        <v>44682</v>
+        <v>44713</v>
       </c>
       <c r="B43" s="4">
-        <v>802</v>
+        <v>1165</v>
       </c>
       <c r="C43" s="4">
-        <v>805</v>
+        <v>960</v>
       </c>
     </row>
     <row r="44" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="6">
-        <v>44713</v>
+        <v>44743</v>
       </c>
       <c r="B44" s="4">
-        <v>1165</v>
+        <v>1336</v>
       </c>
       <c r="C44" s="4">
-        <v>960</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="45" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="6">
-        <v>44743</v>
+        <v>44774</v>
       </c>
       <c r="B45" s="4">
-        <v>1336</v>
+        <v>1550</v>
       </c>
       <c r="C45" s="4">
-        <v>1344</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
-        <v>44774</v>
+        <v>44805</v>
       </c>
       <c r="B46" s="4">
-        <v>1550</v>
+        <v>1753</v>
       </c>
       <c r="C46" s="4">
-        <v>1427</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
-        <v>44805</v>
+        <v>44835</v>
       </c>
       <c r="B47" s="4">
-        <v>1753</v>
+        <v>1570</v>
       </c>
       <c r="C47" s="4">
-        <v>1540</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="6">
-        <v>44835</v>
+        <v>44866</v>
       </c>
       <c r="B48" s="4">
-        <v>1570</v>
+        <v>1333</v>
       </c>
       <c r="C48" s="4">
-        <v>1682</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="6">
-        <v>44866</v>
+        <v>44896</v>
       </c>
       <c r="B49" s="4">
-        <v>1333</v>
+        <v>1250</v>
       </c>
       <c r="C49" s="4">
-        <v>1413</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="6">
-        <v>44896</v>
+        <v>44927</v>
       </c>
       <c r="B50" s="4">
-        <v>1250</v>
+        <v>1216</v>
       </c>
       <c r="C50" s="4">
-        <v>1294</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="6">
-        <v>44927</v>
+        <v>44958</v>
       </c>
       <c r="B51" s="4">
-        <v>1216</v>
+        <v>1765</v>
       </c>
       <c r="C51" s="4">
-        <v>1130</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="6">
-        <v>44958</v>
+        <v>44986</v>
       </c>
       <c r="B52" s="4">
-        <v>1765</v>
+        <v>1917</v>
       </c>
       <c r="C52" s="4">
-        <v>1505</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="6">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="B53" s="4">
-        <v>1917</v>
+        <v>1757</v>
       </c>
       <c r="C53" s="4">
-        <v>1796</v>
-      </c>
+        <v>1892</v>
+      </c>
+      <c r="F53" s="8"/>
     </row>
     <row r="54" spans="1:6" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="6">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="B54" s="4">
-        <v>1757</v>
+        <v>1911</v>
       </c>
       <c r="C54" s="4">
-        <v>1892</v>
+        <v>1780</v>
       </c>
       <c r="F54" s="8"/>
     </row>
-    <row r="55" spans="1:6" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="6">
-        <v>45047</v>
-      </c>
-      <c r="B55" s="4">
-        <v>1911</v>
-      </c>
-      <c r="C55" s="4">
-        <v>1780</v>
-      </c>
-      <c r="F55" s="8"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>